<commit_message>
#imp : active generate-list
</commit_message>
<xml_diff>
--- a/public/Vcard_template.xlsx
+++ b/public/Vcard_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vn.ngockhoe.le\Documents\Keppel\2023_Q4\bz_Vcard\bz-vcard_v4\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vn.ngockhoe.le\Documents\Keppel\2023_Q4\bz_Vcard\react_vCard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E18EF3-95FB-4EBF-A17E-0C08402530FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C22FA5-465D-4CAD-93FD-14FBE19E1A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31515" yWindow="1530" windowWidth="20730" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,74 +25,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
-  <si>
-    <t>84 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>Nguyen Duc Minh</t>
-  </si>
-  <si>
-    <t>nguyendm@keppel.com</t>
-  </si>
-  <si>
-    <t>+84 936 133 037</t>
-  </si>
-  <si>
-    <t>https://keppel.com</t>
-  </si>
-  <si>
-    <t>Keppel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>https://picsum.photos/200/300</t>
   </si>
   <si>
-    <t>Managing Director,Head of Business Development,Real Estate Division (VietNam)</t>
-  </si>
-  <si>
-    <t>85 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>+84 936 133 038</t>
-  </si>
-  <si>
     <t>https://picsum.photos/200/301</t>
   </si>
   <si>
-    <t>86 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>+84 936 133 039</t>
-  </si>
-  <si>
     <t>https://picsum.photos/200/302</t>
   </si>
   <si>
-    <t>87 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>+84 936 133 040</t>
-  </si>
-  <si>
     <t>https://picsum.photos/200/303</t>
   </si>
   <si>
-    <t>88 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>+84 936 133 041</t>
-  </si>
-  <si>
     <t>https://picsum.photos/200/304</t>
   </si>
   <si>
-    <t>89 (28) 3821 8000</t>
-  </si>
-  <si>
-    <t>+84 936 133 042</t>
-  </si>
-  <si>
     <t>https://picsum.photos/200/305</t>
   </si>
   <si>
@@ -121,6 +70,45 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>https://www.google.com.vn/?hl=vi</t>
+  </si>
+  <si>
+    <t>Gooogle</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>+84123456887</t>
+  </si>
+  <si>
+    <t>84 (28)12345678</t>
+  </si>
+  <si>
+    <t>85 (28)12345678</t>
+  </si>
+  <si>
+    <t>86 (28)12345678</t>
+  </si>
+  <si>
+    <t>87 (28)12345678</t>
+  </si>
+  <si>
+    <t>88 (28)12345678</t>
+  </si>
+  <si>
+    <t>89 (28)12345678</t>
+  </si>
+  <si>
+    <t>Head of IT</t>
+  </si>
+  <si>
+    <t>Nguyen Van A</t>
+  </si>
+  <si>
+    <t>Nguyen Van B</t>
   </si>
 </sst>
 </file>
@@ -527,7 +515,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,67 +525,67 @@
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>0</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -605,144 +593,144 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -751,21 +739,13 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{81C40FF1-6C2B-4989-8581-B37C9CDA462A}"/>
     <hyperlink ref="G2" r:id="rId2" xr:uid="{69B76784-BF31-404D-9B4F-E9232DA153F3}"/>
     <hyperlink ref="I2" r:id="rId3" xr:uid="{9E530181-95FC-4A35-A7D2-B60CB1B2B890}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{1FB826A3-7944-427C-9D36-09BFC01FAE79}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{05219FDF-7304-46ED-99F8-2721176DC2D5}"/>
-    <hyperlink ref="D5" r:id="rId6" xr:uid="{1B6A4B81-4E0C-4A78-BD6E-29B7454C1851}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{FD5849B5-5C6F-4CCC-866E-832D6B641BA0}"/>
-    <hyperlink ref="D7" r:id="rId8" xr:uid="{FBF9E37F-BECF-430D-A7D2-F409B32004B0}"/>
-    <hyperlink ref="G3" r:id="rId9" xr:uid="{510CEAD2-76E8-472B-AE9D-072A1DFDD442}"/>
-    <hyperlink ref="G4" r:id="rId10" xr:uid="{53E29213-910A-4F48-951B-A7567702B0EA}"/>
-    <hyperlink ref="G5" r:id="rId11" xr:uid="{72440F81-29DD-4738-8359-E52B103FBCB3}"/>
-    <hyperlink ref="G6" r:id="rId12" xr:uid="{8DAE2271-EC05-4ED7-A9A3-9EFA6EC37A1C}"/>
-    <hyperlink ref="G7" r:id="rId13" xr:uid="{A89433B4-E77D-43E3-A8B1-E4A93126CA8A}"/>
-    <hyperlink ref="I3" r:id="rId14" display="https://picsum.photos/200/300" xr:uid="{7F33998C-BFF7-424E-A376-A5F46A6BC5BF}"/>
-    <hyperlink ref="I4" r:id="rId15" display="https://picsum.photos/200/300" xr:uid="{F6F66B40-C001-4AF4-ADE3-1629C8B16E25}"/>
-    <hyperlink ref="I5" r:id="rId16" display="https://picsum.photos/200/300" xr:uid="{D6E5F94B-A68A-417A-B670-45F6987B3EED}"/>
-    <hyperlink ref="I6" r:id="rId17" display="https://picsum.photos/200/300" xr:uid="{785BD75A-65CE-4E0E-99FE-752B5C2BED6B}"/>
-    <hyperlink ref="I7" r:id="rId18" display="https://picsum.photos/200/300" xr:uid="{212AE502-0B8C-4286-BAE9-EE0CB01D0D7F}"/>
+    <hyperlink ref="I3" r:id="rId4" display="https://picsum.photos/200/300" xr:uid="{7F33998C-BFF7-424E-A376-A5F46A6BC5BF}"/>
+    <hyperlink ref="I4" r:id="rId5" display="https://picsum.photos/200/300" xr:uid="{F6F66B40-C001-4AF4-ADE3-1629C8B16E25}"/>
+    <hyperlink ref="I5" r:id="rId6" display="https://picsum.photos/200/300" xr:uid="{D6E5F94B-A68A-417A-B670-45F6987B3EED}"/>
+    <hyperlink ref="I6" r:id="rId7" display="https://picsum.photos/200/300" xr:uid="{785BD75A-65CE-4E0E-99FE-752B5C2BED6B}"/>
+    <hyperlink ref="I7" r:id="rId8" display="https://picsum.photos/200/300" xr:uid="{212AE502-0B8C-4286-BAE9-EE0CB01D0D7F}"/>
+    <hyperlink ref="G3:G7" r:id="rId9" display="https://www.google.com.vn/?hl=vi" xr:uid="{8533C874-6F4D-4BE0-947B-BDB0612B5128}"/>
+    <hyperlink ref="D3:D7" r:id="rId10" display="abcd@gmail.com" xr:uid="{BD76C501-0D38-4BA7-A11C-6C7257830C1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>